<commit_message>
SendKeyEvent() now uses TranslateAhkCode()
</commit_message>
<xml_diff>
--- a/C#/AutoHotInterception/KeyCode notes.xlsx
+++ b/C#/AutoHotInterception/KeyCode notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Code\GitHub\Mine\AHK+C#\AutoHotInterception\C#\AutoHotInterception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353AD7A1-C9F3-456D-9311-5BDB35E479B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF353844-7E17-48F5-98BB-F833F0F28AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-375" windowWidth="29040" windowHeight="17790" xr2:uid="{12F25D4D-4D4F-43AE-975E-852A909327AE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -195,6 +195,9 @@
   <si>
     <t>ext press, key press, key release, ext release
 (Ext code only sent if Numlock is off)</t>
+  </si>
+  <si>
+    <t>PrintScreen</t>
   </si>
 </sst>
 </file>
@@ -642,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B806E1-24CF-4FCD-AA4B-22626E9391BA}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,7 +732,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C22" si="0" xml:space="preserve"> B3 + 256</f>
+        <f t="shared" ref="C3:C23" si="0" xml:space="preserve"> B3 + 256</f>
         <v>285</v>
       </c>
       <c r="D3" s="12">
@@ -786,149 +789,136 @@
     </row>
     <row r="6" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="12">
+        <v>55</v>
+      </c>
+      <c r="C6" s="12">
+        <v>311</v>
+      </c>
+      <c r="D6" s="12">
+        <v>311</v>
+      </c>
+      <c r="E6" s="12">
+        <v>2</v>
+      </c>
+      <c r="F6" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B7" s="12">
         <v>56</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D7" s="12">
         <v>312</v>
       </c>
-      <c r="E6" s="12">
-        <v>2</v>
-      </c>
-      <c r="F6" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="E7" s="12">
+        <v>2</v>
+      </c>
+      <c r="F7" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B8" s="19">
         <v>69</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C8" s="19">
         <f t="shared" si="0"/>
         <v>325</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D8" s="19">
         <v>325</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E8" s="19">
         <v>0</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F8" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+    <row r="9" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B9" s="17">
         <v>69</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C9" s="17">
         <f t="shared" si="0"/>
         <v>325</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D9" s="17">
         <v>69</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E9" s="17">
         <v>0</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F9" s="17">
         <v>1</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G9" s="17">
         <v>29</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I9" s="17">
         <v>4</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J9" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+    <row r="10" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B10" s="12">
         <v>70</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C10" s="12">
         <f t="shared" si="0"/>
         <v>326</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D10" s="12">
         <v>326</v>
       </c>
-      <c r="E9" s="12">
-        <v>2</v>
-      </c>
-      <c r="F9" s="12">
-        <v>3</v>
-      </c>
-      <c r="K9" s="12" t="s">
+      <c r="E10" s="12">
+        <v>2</v>
+      </c>
+      <c r="F10" s="12">
+        <v>3</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="13">
-        <v>71</v>
-      </c>
-      <c r="C10" s="13">
-        <f t="shared" si="0"/>
-        <v>327</v>
-      </c>
-      <c r="D10" s="13">
-        <v>327</v>
-      </c>
-      <c r="E10" s="13">
-        <v>2</v>
-      </c>
-      <c r="F10" s="13">
-        <v>3</v>
-      </c>
-      <c r="G10" s="13">
-        <v>42</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="13">
-        <v>2</v>
-      </c>
-      <c r="J10" s="13">
-        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="13">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="13">
         <f t="shared" si="0"/>
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D11" s="13">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E11" s="13">
         <v>2</v>
@@ -951,17 +941,17 @@
     </row>
     <row r="12" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="13">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="13">
         <f t="shared" si="0"/>
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D12" s="13">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E12" s="13">
         <v>2</v>
@@ -984,17 +974,17 @@
     </row>
     <row r="13" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="13">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" s="13">
         <f t="shared" si="0"/>
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D13" s="13">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E13" s="13">
         <v>2</v>
@@ -1017,17 +1007,17 @@
     </row>
     <row r="14" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="13">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" s="13">
         <f t="shared" si="0"/>
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D14" s="13">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E14" s="13">
         <v>2</v>
@@ -1050,17 +1040,17 @@
     </row>
     <row r="15" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="13">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" s="13">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D15" s="13">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E15" s="13">
         <v>2</v>
@@ -1083,17 +1073,17 @@
     </row>
     <row r="16" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="13">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="13">
         <f t="shared" si="0"/>
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D16" s="13">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E16" s="13">
         <v>2</v>
@@ -1116,17 +1106,17 @@
     </row>
     <row r="17" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="13">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="13">
         <f t="shared" si="0"/>
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D17" s="13">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E17" s="13">
         <v>2</v>
@@ -1149,17 +1139,17 @@
     </row>
     <row r="18" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="13">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="13">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D18" s="13">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E18" s="13">
         <v>2</v>
@@ -1182,17 +1172,17 @@
     </row>
     <row r="19" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="13">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" s="13">
         <f t="shared" si="0"/>
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D19" s="13">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E19" s="13">
         <v>2</v>
@@ -1213,40 +1203,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="12">
-        <v>91</v>
-      </c>
-      <c r="C20" s="12">
-        <f t="shared" si="0"/>
-        <v>347</v>
-      </c>
-      <c r="D20" s="12">
-        <v>347</v>
-      </c>
-      <c r="E20" s="12">
-        <v>2</v>
-      </c>
-      <c r="F20" s="12">
+    <row r="20" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="13">
+        <v>83</v>
+      </c>
+      <c r="C20" s="13">
+        <f t="shared" si="0"/>
+        <v>339</v>
+      </c>
+      <c r="D20" s="13">
+        <v>339</v>
+      </c>
+      <c r="E20" s="13">
+        <v>2</v>
+      </c>
+      <c r="F20" s="13">
+        <v>3</v>
+      </c>
+      <c r="G20" s="13">
+        <v>42</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="13">
+        <v>2</v>
+      </c>
+      <c r="J20" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="12">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="12">
         <f t="shared" si="0"/>
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D21" s="12">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E21" s="12">
         <v>2</v>
@@ -1257,129 +1259,150 @@
     </row>
     <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="12">
+        <v>92</v>
+      </c>
+      <c r="C22" s="12">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
+      <c r="D22" s="12">
+        <v>348</v>
+      </c>
+      <c r="E22" s="12">
+        <v>2</v>
+      </c>
+      <c r="F22" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B23" s="12">
         <v>93</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C23" s="12">
         <f t="shared" si="0"/>
         <v>349</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D23" s="12">
         <v>349</v>
       </c>
-      <c r="E22" s="12">
-        <v>2</v>
-      </c>
-      <c r="F22" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D24" s="4"/>
-      <c r="I24" t="s">
+      <c r="E23" s="12">
+        <v>2</v>
+      </c>
+      <c r="F23" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D25" s="4"/>
+      <c r="I25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C25" s="2"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="15" t="s">
+    <row r="26" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C26" s="2"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="G26" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H26" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="I26" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="J25" s="16" t="s">
+      <c r="J26" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K26" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D26" s="8"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D27" s="8"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="1"/>
       <c r="G27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H27">
         <v>256</v>
       </c>
-      <c r="I27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J27" t="s">
+    </row>
+    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D28" s="8"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D28" s="8"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H28">
         <v>256</v>
       </c>
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" t="s">
+        <v>31</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D29" s="8"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="6" t="s">
+      <c r="F29" s="3"/>
+      <c r="G29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29" t="s">
-        <v>25</v>
-      </c>
-      <c r="J29" t="s">
-        <v>33</v>
-      </c>
-      <c r="K29" t="s">
-        <v>35</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D30" s="8"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="8"/>
-      <c r="K31" s="14" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D32" s="8"/>
-      <c r="K32" t="s">
+      <c r="K32" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D33" s="8"/>
+      <c r="K33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="11:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="K33" s="4" t="s">
+    <row r="34" spans="4:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="K34" s="4" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>